<commit_message>
Outlined methods and tables
</commit_message>
<xml_diff>
--- a/1_data/tables.xlsx
+++ b/1_data/tables.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Projects\generic_project\1_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/william_russell_mcgill_ca/Documents/Projects/opal-assessment/1_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC76095-3DD5-4ADC-A9C8-8CEF9F69B11E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{7BC76095-3DD5-4ADC-A9C8-8CEF9F69B11E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED1841EA-9D2B-6D40-B490-D900CD7571EB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{FD511D9A-EB76-4ABE-81DE-0F0E048ADAAB}"/>
+    <workbookView xWindow="38400" yWindow="4760" windowWidth="28800" windowHeight="17500" xr2:uid="{FD511D9A-EB76-4ABE-81DE-0F0E048ADAAB}"/>
   </bookViews>
   <sheets>
-    <sheet name="sample" sheetId="1" r:id="rId1"/>
+    <sheet name="Datasets" sheetId="1" r:id="rId1"/>
+    <sheet name="Controls" sheetId="2" r:id="rId2"/>
+    <sheet name="Outcomes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,46 +36,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
-  <si>
-    <t>col1</t>
-  </si>
-  <si>
-    <t>col2</t>
-  </si>
-  <si>
-    <t>subhead</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>[@Keane2018]</t>
-  </si>
-  <si>
-    <t>Yes^[Footnote 2]</t>
-  </si>
-  <si>
-    <t>[@Langham2018a]^[Footnote 1]</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Example variables</t>
+  </si>
+  <si>
+    <t>Opal usage</t>
+  </si>
+  <si>
+    <t>Visit data</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Description/preprocessing notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +75,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -426,75 +417,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6B55D8-F496-4084-B55D-ABB6EB68893D}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1E8BA3-6747-C943-BFE2-A77AD5E6E438}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="31.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
+      <c r="B1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D571A6-5F0B-354E-8480-7FE21F418F6C}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>